<commit_message>
add some notebook for analyse data
</commit_message>
<xml_diff>
--- a/docs/model_results_best.xlsx
+++ b/docs/model_results_best.xlsx
@@ -639,7 +639,7 @@
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -910,8 +910,8 @@
       <c r="A16" t="s">
         <v>47</v>
       </c>
-      <c r="B16" t="s">
-        <v>48</v>
+      <c r="B16" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="C16" t="s">
         <v>49</v>
@@ -927,8 +927,8 @@
       <c r="A17" t="s">
         <v>50</v>
       </c>
-      <c r="B17" t="s">
-        <v>51</v>
+      <c r="B17" s="0" t="s">
+        <v>24</v>
       </c>
       <c r="C17" t="s">
         <v>52</v>
@@ -944,8 +944,8 @@
       <c r="A18" t="s">
         <v>53</v>
       </c>
-      <c r="B18" t="s">
-        <v>54</v>
+      <c r="B18" s="0" t="s">
+        <v>27</v>
       </c>
       <c r="C18" t="s">
         <v>55</v>

</xml_diff>